<commit_message>
Update lotto data (2026-01-10 15:36)
</commit_message>
<xml_diff>
--- a/lotto_prob.xlsx
+++ b/lotto_prob.xlsx
@@ -946,7 +946,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -1149,7 +1149,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1204,7 +1204,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1549,7 +1549,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L1300"/>
+  <dimension ref="A1:L1301"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A1200" activePane="bottomLeft" state="frozen"/>
@@ -33554,25 +33554,48 @@
       <c r="A1299" s="34" t="n"/>
     </row>
     <row r="1300">
-      <c r="A1300" t="n">
+      <c r="A1300" s="30" t="n">
         <v>1206</v>
       </c>
-      <c r="B1300" t="n">
+      <c r="B1300" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="C1300" t="n">
+      <c r="C1300" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="D1300" t="n">
+      <c r="D1300" s="30" t="n">
         <v>17</v>
       </c>
-      <c r="E1300" t="n">
+      <c r="E1300" s="30" t="n">
         <v>26</v>
       </c>
-      <c r="F1300" t="n">
+      <c r="F1300" s="30" t="n">
         <v>27</v>
       </c>
-      <c r="G1300" t="n">
+      <c r="G1300" s="30" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="n">
+        <v>1207</v>
+      </c>
+      <c r="B1301" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1301" t="n">
+        <v>3</v>
+      </c>
+      <c r="D1301" t="n">
+        <v>17</v>
+      </c>
+      <c r="E1301" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1301" t="n">
+        <v>27</v>
+      </c>
+      <c r="G1301" t="n">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update lotto data (2026-01-24 13:07)
</commit_message>
<xml_diff>
--- a/lotto_prob.xlsx
+++ b/lotto_prob.xlsx
@@ -905,7 +905,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -1108,7 +1108,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1163,7 +1163,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -47401,25 +47401,25 @@
       <c r="A1208" s="31" t="n">
         <v>1207</v>
       </c>
-      <c r="B1208" t="n">
+      <c r="B1208" s="27" t="n">
         <v>10</v>
       </c>
-      <c r="C1208" t="n">
+      <c r="C1208" s="27" t="n">
         <v>22</v>
       </c>
-      <c r="D1208" t="n">
+      <c r="D1208" s="27" t="n">
         <v>24</v>
       </c>
-      <c r="E1208" t="n">
+      <c r="E1208" s="27" t="n">
         <v>27</v>
       </c>
-      <c r="F1208" t="n">
+      <c r="F1208" s="27" t="n">
         <v>38</v>
       </c>
-      <c r="G1208" t="n">
+      <c r="G1208" s="27" t="n">
         <v>45</v>
       </c>
-      <c r="H1208" t="n">
+      <c r="H1208" s="27" t="n">
         <v>11</v>
       </c>
       <c r="J1208" s="27">
@@ -47436,7 +47436,30 @@
       </c>
     </row>
     <row r="1209" ht="13.8" customHeight="1" s="28">
-      <c r="A1209" s="31" t="n"/>
+      <c r="A1209" s="31" t="n">
+        <v>1208</v>
+      </c>
+      <c r="B1209" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1209" t="n">
+        <v>27</v>
+      </c>
+      <c r="D1209" t="n">
+        <v>30</v>
+      </c>
+      <c r="E1209" t="n">
+        <v>36</v>
+      </c>
+      <c r="F1209" t="n">
+        <v>38</v>
+      </c>
+      <c r="G1209" t="n">
+        <v>42</v>
+      </c>
+      <c r="H1209" t="n">
+        <v>25</v>
+      </c>
       <c r="J1209" s="27">
         <f>SUMPRODUCT(COUNTIFS(확률!$J$2:$J$46, 원본!B1209:G1209, 확률!$M$2:$M$46, "&lt;=20"))</f>
         <v/>

</xml_diff>

<commit_message>
Update lotto data (2026-01-31 13:22)
</commit_message>
<xml_diff>
--- a/lotto_prob.xlsx
+++ b/lotto_prob.xlsx
@@ -47439,25 +47439,25 @@
       <c r="A1209" s="31" t="n">
         <v>1208</v>
       </c>
-      <c r="B1209" t="n">
+      <c r="B1209" s="27" t="n">
         <v>6</v>
       </c>
-      <c r="C1209" t="n">
+      <c r="C1209" s="27" t="n">
         <v>27</v>
       </c>
-      <c r="D1209" t="n">
+      <c r="D1209" s="27" t="n">
         <v>30</v>
       </c>
-      <c r="E1209" t="n">
+      <c r="E1209" s="27" t="n">
         <v>36</v>
       </c>
-      <c r="F1209" t="n">
+      <c r="F1209" s="27" t="n">
         <v>38</v>
       </c>
-      <c r="G1209" t="n">
+      <c r="G1209" s="27" t="n">
         <v>42</v>
       </c>
-      <c r="H1209" t="n">
+      <c r="H1209" s="27" t="n">
         <v>25</v>
       </c>
       <c r="J1209" s="27">
@@ -47474,7 +47474,30 @@
       </c>
     </row>
     <row r="1210" ht="13.8" customHeight="1" s="28">
-      <c r="A1210" s="31" t="n"/>
+      <c r="A1210" s="31" t="n">
+        <v>1209</v>
+      </c>
+      <c r="B1210" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1210" t="n">
+        <v>17</v>
+      </c>
+      <c r="D1210" t="n">
+        <v>20</v>
+      </c>
+      <c r="E1210" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1210" t="n">
+        <v>37</v>
+      </c>
+      <c r="G1210" t="n">
+        <v>39</v>
+      </c>
+      <c r="H1210" t="n">
+        <v>24</v>
+      </c>
       <c r="J1210" s="27">
         <f>SUMPRODUCT(COUNTIFS(확률!$J$2:$J$46, 원본!B1210:G1210, 확률!$M$2:$M$46, "&lt;=20"))</f>
         <v/>

</xml_diff>

<commit_message>
Update lotto data (2026-02-07 13:25)
</commit_message>
<xml_diff>
--- a/lotto_prob.xlsx
+++ b/lotto_prob.xlsx
@@ -47477,25 +47477,25 @@
       <c r="A1210" s="31" t="n">
         <v>1209</v>
       </c>
-      <c r="B1210" t="n">
+      <c r="B1210" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="C1210" t="n">
+      <c r="C1210" s="27" t="n">
         <v>17</v>
       </c>
-      <c r="D1210" t="n">
+      <c r="D1210" s="27" t="n">
         <v>20</v>
       </c>
-      <c r="E1210" t="n">
+      <c r="E1210" s="27" t="n">
         <v>35</v>
       </c>
-      <c r="F1210" t="n">
+      <c r="F1210" s="27" t="n">
         <v>37</v>
       </c>
-      <c r="G1210" t="n">
+      <c r="G1210" s="27" t="n">
         <v>39</v>
       </c>
-      <c r="H1210" t="n">
+      <c r="H1210" s="27" t="n">
         <v>24</v>
       </c>
       <c r="J1210" s="27">
@@ -47512,7 +47512,30 @@
       </c>
     </row>
     <row r="1211" ht="13.8" customHeight="1" s="28">
-      <c r="A1211" s="31" t="n"/>
+      <c r="A1211" s="31" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B1211" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1211" t="n">
+        <v>7</v>
+      </c>
+      <c r="D1211" t="n">
+        <v>9</v>
+      </c>
+      <c r="E1211" t="n">
+        <v>17</v>
+      </c>
+      <c r="F1211" t="n">
+        <v>27</v>
+      </c>
+      <c r="G1211" t="n">
+        <v>38</v>
+      </c>
+      <c r="H1211" t="n">
+        <v>31</v>
+      </c>
       <c r="J1211" s="27">
         <f>SUMPRODUCT(COUNTIFS(확률!$J$2:$J$46, 원본!B1211:G1211, 확률!$M$2:$M$46, "&lt;=20"))</f>
         <v/>

</xml_diff>

<commit_message>
Update lotto data (2026-02-14 13:25)
</commit_message>
<xml_diff>
--- a/lotto_prob.xlsx
+++ b/lotto_prob.xlsx
@@ -47515,25 +47515,25 @@
       <c r="A1211" s="31" t="n">
         <v>1210</v>
       </c>
-      <c r="B1211" t="n">
+      <c r="B1211" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="C1211" t="n">
+      <c r="C1211" s="27" t="n">
         <v>7</v>
       </c>
-      <c r="D1211" t="n">
+      <c r="D1211" s="27" t="n">
         <v>9</v>
       </c>
-      <c r="E1211" t="n">
+      <c r="E1211" s="27" t="n">
         <v>17</v>
       </c>
-      <c r="F1211" t="n">
+      <c r="F1211" s="27" t="n">
         <v>27</v>
       </c>
-      <c r="G1211" t="n">
+      <c r="G1211" s="27" t="n">
         <v>38</v>
       </c>
-      <c r="H1211" t="n">
+      <c r="H1211" s="27" t="n">
         <v>31</v>
       </c>
       <c r="J1211" s="27">
@@ -47550,7 +47550,30 @@
       </c>
     </row>
     <row r="1212" ht="13.8" customHeight="1" s="28">
-      <c r="A1212" s="31" t="n"/>
+      <c r="A1212" s="31" t="n">
+        <v>1211</v>
+      </c>
+      <c r="B1212" t="n">
+        <v>23</v>
+      </c>
+      <c r="C1212" t="n">
+        <v>26</v>
+      </c>
+      <c r="D1212" t="n">
+        <v>27</v>
+      </c>
+      <c r="E1212" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1212" t="n">
+        <v>38</v>
+      </c>
+      <c r="G1212" t="n">
+        <v>40</v>
+      </c>
+      <c r="H1212" t="n">
+        <v>10</v>
+      </c>
       <c r="J1212" s="27">
         <f>SUMPRODUCT(COUNTIFS(확률!$J$2:$J$46, 원본!B1212:G1212, 확률!$M$2:$M$46, "&lt;=20"))</f>
         <v/>

</xml_diff>

<commit_message>
Update lotto data (2026-02-21 13:24)
</commit_message>
<xml_diff>
--- a/lotto_prob.xlsx
+++ b/lotto_prob.xlsx
@@ -47553,25 +47553,25 @@
       <c r="A1212" s="31" t="n">
         <v>1211</v>
       </c>
-      <c r="B1212" t="n">
+      <c r="B1212" s="27" t="n">
         <v>23</v>
       </c>
-      <c r="C1212" t="n">
+      <c r="C1212" s="27" t="n">
         <v>26</v>
       </c>
-      <c r="D1212" t="n">
+      <c r="D1212" s="27" t="n">
         <v>27</v>
       </c>
-      <c r="E1212" t="n">
+      <c r="E1212" s="27" t="n">
         <v>35</v>
       </c>
-      <c r="F1212" t="n">
+      <c r="F1212" s="27" t="n">
         <v>38</v>
       </c>
-      <c r="G1212" t="n">
+      <c r="G1212" s="27" t="n">
         <v>40</v>
       </c>
-      <c r="H1212" t="n">
+      <c r="H1212" s="27" t="n">
         <v>10</v>
       </c>
       <c r="J1212" s="27">
@@ -47588,7 +47588,30 @@
       </c>
     </row>
     <row r="1213" ht="13.8" customHeight="1" s="28">
-      <c r="A1213" s="31" t="n"/>
+      <c r="A1213" s="31" t="n">
+        <v>1212</v>
+      </c>
+      <c r="B1213" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1213" t="n">
+        <v>8</v>
+      </c>
+      <c r="D1213" t="n">
+        <v>25</v>
+      </c>
+      <c r="E1213" t="n">
+        <v>31</v>
+      </c>
+      <c r="F1213" t="n">
+        <v>41</v>
+      </c>
+      <c r="G1213" t="n">
+        <v>44</v>
+      </c>
+      <c r="H1213" t="n">
+        <v>45</v>
+      </c>
       <c r="J1213" s="27">
         <f>SUMPRODUCT(COUNTIFS(확률!$J$2:$J$46, 원본!B1213:G1213, 확률!$M$2:$M$46, "&lt;=20"))</f>
         <v/>

</xml_diff>

<commit_message>
Update lotto data (2026-02-28 13:11)
</commit_message>
<xml_diff>
--- a/lotto_prob.xlsx
+++ b/lotto_prob.xlsx
@@ -47591,25 +47591,25 @@
       <c r="A1213" s="31" t="n">
         <v>1212</v>
       </c>
-      <c r="B1213" t="n">
+      <c r="B1213" s="27" t="n">
         <v>5</v>
       </c>
-      <c r="C1213" t="n">
+      <c r="C1213" s="27" t="n">
         <v>8</v>
       </c>
-      <c r="D1213" t="n">
+      <c r="D1213" s="27" t="n">
         <v>25</v>
       </c>
-      <c r="E1213" t="n">
+      <c r="E1213" s="27" t="n">
         <v>31</v>
       </c>
-      <c r="F1213" t="n">
+      <c r="F1213" s="27" t="n">
         <v>41</v>
       </c>
-      <c r="G1213" t="n">
+      <c r="G1213" s="27" t="n">
         <v>44</v>
       </c>
-      <c r="H1213" t="n">
+      <c r="H1213" s="27" t="n">
         <v>45</v>
       </c>
       <c r="J1213" s="27">
@@ -47626,7 +47626,30 @@
       </c>
     </row>
     <row r="1214" ht="13.8" customHeight="1" s="28">
-      <c r="A1214" s="31" t="n"/>
+      <c r="A1214" s="31" t="n">
+        <v>1213</v>
+      </c>
+      <c r="B1214" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1214" t="n">
+        <v>11</v>
+      </c>
+      <c r="D1214" t="n">
+        <v>25</v>
+      </c>
+      <c r="E1214" t="n">
+        <v>27</v>
+      </c>
+      <c r="F1214" t="n">
+        <v>36</v>
+      </c>
+      <c r="G1214" t="n">
+        <v>38</v>
+      </c>
+      <c r="H1214" t="n">
+        <v>2</v>
+      </c>
       <c r="J1214" s="27">
         <f>SUMPRODUCT(COUNTIFS(확률!$J$2:$J$46, 원본!B1214:G1214, 확률!$M$2:$M$46, "&lt;=20"))</f>
         <v/>

</xml_diff>